<commit_message>
Changed coding of significant column
</commit_message>
<xml_diff>
--- a/Regulators/regulator_variation_summary.xlsx
+++ b/Regulators/regulator_variation_summary.xlsx
@@ -1568,9 +1568,7 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
+      <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
     </row>
@@ -1713,9 +1711,7 @@
       <c r="B23" t="n">
         <v>0</v>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
+      <c r="C23"/>
       <c r="D23" t="s">
         <v>6</v>
       </c>
@@ -1728,9 +1724,7 @@
       <c r="B24" t="n">
         <v>0</v>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
+      <c r="C24"/>
       <c r="D24" t="s">
         <v>9</v>
       </c>
@@ -1743,9 +1737,7 @@
       <c r="B25" t="n">
         <v>0</v>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
+      <c r="C25"/>
       <c r="D25" t="s">
         <v>9</v>
       </c>
@@ -1843,9 +1835,7 @@
       <c r="B31" t="n">
         <v>0</v>
       </c>
-      <c r="C31" t="n">
-        <v>1</v>
-      </c>
+      <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
     </row>
@@ -1856,9 +1846,7 @@
       <c r="B32" t="n">
         <v>0</v>
       </c>
-      <c r="C32" t="n">
-        <v>1</v>
-      </c>
+      <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
     </row>
@@ -1869,9 +1857,7 @@
       <c r="B33" t="n">
         <v>0</v>
       </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
+      <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
     </row>
@@ -1933,9 +1919,7 @@
       <c r="B37" t="n">
         <v>0</v>
       </c>
-      <c r="C37" t="n">
-        <v>1</v>
-      </c>
+      <c r="C37"/>
       <c r="D37" t="s">
         <v>13</v>
       </c>
@@ -2216,9 +2200,7 @@
       <c r="B54" t="n">
         <v>0</v>
       </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
+      <c r="C54"/>
       <c r="D54" t="s">
         <v>9</v>
       </c>
@@ -2295,9 +2277,7 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
-      <c r="C59" t="n">
-        <v>1</v>
-      </c>
+      <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
     </row>
@@ -2338,9 +2318,7 @@
       <c r="B62" t="n">
         <v>0</v>
       </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
+      <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
     </row>
@@ -2453,9 +2431,7 @@
       <c r="B69" t="n">
         <v>0</v>
       </c>
-      <c r="C69" t="n">
-        <v>0</v>
-      </c>
+      <c r="C69"/>
       <c r="D69" t="s">
         <v>9</v>
       </c>
@@ -2485,9 +2461,7 @@
       <c r="B71" t="n">
         <v>0</v>
       </c>
-      <c r="C71" t="n">
-        <v>0</v>
-      </c>
+      <c r="C71"/>
       <c r="D71" t="s">
         <v>13</v>
       </c>
@@ -2517,9 +2491,7 @@
       <c r="B73" t="n">
         <v>0</v>
       </c>
-      <c r="C73" t="n">
-        <v>0</v>
-      </c>
+      <c r="C73"/>
       <c r="D73" t="s">
         <v>9</v>
       </c>
@@ -2651,9 +2623,7 @@
       <c r="B81" t="n">
         <v>0</v>
       </c>
-      <c r="C81" t="n">
-        <v>0</v>
-      </c>
+      <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
     </row>
@@ -2664,9 +2634,7 @@
       <c r="B82" t="n">
         <v>0</v>
       </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
+      <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
     </row>
@@ -2690,9 +2658,7 @@
       <c r="B84" t="n">
         <v>0</v>
       </c>
-      <c r="C84" t="n">
-        <v>0</v>
-      </c>
+      <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
     </row>
@@ -2703,9 +2669,7 @@
       <c r="B85" t="n">
         <v>0</v>
       </c>
-      <c r="C85" t="n">
-        <v>0</v>
-      </c>
+      <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
     </row>
@@ -2784,9 +2748,7 @@
       <c r="B90" t="n">
         <v>0</v>
       </c>
-      <c r="C90" t="n">
-        <v>0</v>
-      </c>
+      <c r="C90"/>
       <c r="D90" t="s">
         <v>9</v>
       </c>
@@ -2867,9 +2829,7 @@
       <c r="B95" t="n">
         <v>0</v>
       </c>
-      <c r="C95" t="n">
-        <v>0</v>
-      </c>
+      <c r="C95"/>
       <c r="D95" t="s">
         <v>15</v>
       </c>
@@ -2899,9 +2859,7 @@
       <c r="B97" t="n">
         <v>0</v>
       </c>
-      <c r="C97" t="n">
-        <v>0</v>
-      </c>
+      <c r="C97"/>
       <c r="D97" t="s">
         <v>15</v>
       </c>
@@ -2948,9 +2906,7 @@
       <c r="B100" t="n">
         <v>0</v>
       </c>
-      <c r="C100" t="n">
-        <v>1</v>
-      </c>
+      <c r="C100"/>
       <c r="D100" t="s">
         <v>9</v>
       </c>
@@ -2980,9 +2936,7 @@
       <c r="B102" t="n">
         <v>0</v>
       </c>
-      <c r="C102" t="n">
-        <v>1</v>
-      </c>
+      <c r="C102"/>
       <c r="D102" t="s">
         <v>9</v>
       </c>
@@ -2995,9 +2949,7 @@
       <c r="B103" t="n">
         <v>0</v>
       </c>
-      <c r="C103" t="n">
-        <v>1</v>
-      </c>
+      <c r="C103"/>
       <c r="D103" t="s">
         <v>9</v>
       </c>
@@ -3010,9 +2962,7 @@
       <c r="B104" t="n">
         <v>0</v>
       </c>
-      <c r="C104" t="n">
-        <v>1</v>
-      </c>
+      <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
     </row>
@@ -3036,9 +2986,7 @@
       <c r="B106" t="n">
         <v>0</v>
       </c>
-      <c r="C106" t="n">
-        <v>0</v>
-      </c>
+      <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
     </row>
@@ -3049,9 +2997,7 @@
       <c r="B107" t="n">
         <v>0</v>
       </c>
-      <c r="C107" t="n">
-        <v>0</v>
-      </c>
+      <c r="C107"/>
       <c r="D107"/>
       <c r="E107"/>
     </row>
@@ -3062,9 +3008,7 @@
       <c r="B108" t="n">
         <v>0</v>
       </c>
-      <c r="C108" t="n">
-        <v>0</v>
-      </c>
+      <c r="C108"/>
       <c r="D108"/>
       <c r="E108"/>
     </row>
@@ -3088,9 +3032,7 @@
       <c r="B110" t="n">
         <v>0</v>
       </c>
-      <c r="C110" t="n">
-        <v>0</v>
-      </c>
+      <c r="C110"/>
       <c r="D110"/>
       <c r="E110"/>
     </row>
@@ -3101,9 +3043,7 @@
       <c r="B111" t="n">
         <v>0</v>
       </c>
-      <c r="C111" t="n">
-        <v>0</v>
-      </c>
+      <c r="C111"/>
       <c r="D111"/>
       <c r="E111"/>
     </row>
@@ -3127,9 +3067,7 @@
       <c r="B113" t="n">
         <v>0</v>
       </c>
-      <c r="C113" t="n">
-        <v>1</v>
-      </c>
+      <c r="C113"/>
       <c r="D113"/>
       <c r="E113"/>
     </row>
@@ -3140,9 +3078,7 @@
       <c r="B114" t="n">
         <v>0</v>
       </c>
-      <c r="C114" t="n">
-        <v>1</v>
-      </c>
+      <c r="C114"/>
       <c r="D114"/>
       <c r="E114"/>
     </row>
@@ -3153,9 +3089,7 @@
       <c r="B115" t="n">
         <v>0</v>
       </c>
-      <c r="C115" t="n">
-        <v>1</v>
-      </c>
+      <c r="C115"/>
       <c r="D115"/>
       <c r="E115"/>
     </row>
@@ -3166,9 +3100,7 @@
       <c r="B116" t="n">
         <v>0</v>
       </c>
-      <c r="C116" t="n">
-        <v>1</v>
-      </c>
+      <c r="C116"/>
       <c r="D116"/>
       <c r="E116"/>
     </row>
@@ -3192,9 +3124,7 @@
       <c r="B118" t="n">
         <v>0</v>
       </c>
-      <c r="C118" t="n">
-        <v>1</v>
-      </c>
+      <c r="C118"/>
       <c r="D118"/>
       <c r="E118"/>
     </row>
@@ -3257,9 +3187,7 @@
       <c r="B123" t="n">
         <v>0</v>
       </c>
-      <c r="C123" t="n">
-        <v>1</v>
-      </c>
+      <c r="C123"/>
       <c r="D123" t="s">
         <v>9</v>
       </c>
@@ -3272,9 +3200,7 @@
       <c r="B124" t="n">
         <v>0</v>
       </c>
-      <c r="C124" t="n">
-        <v>1</v>
-      </c>
+      <c r="C124"/>
       <c r="D124"/>
       <c r="E124"/>
     </row>
@@ -3285,9 +3211,7 @@
       <c r="B125" t="n">
         <v>0</v>
       </c>
-      <c r="C125" t="n">
-        <v>1</v>
-      </c>
+      <c r="C125"/>
       <c r="D125"/>
       <c r="E125"/>
     </row>
@@ -3315,9 +3239,7 @@
       <c r="B127" t="n">
         <v>0</v>
       </c>
-      <c r="C127" t="n">
-        <v>1</v>
-      </c>
+      <c r="C127"/>
       <c r="D127"/>
       <c r="E127"/>
     </row>
@@ -3341,9 +3263,7 @@
       <c r="B129" t="n">
         <v>0</v>
       </c>
-      <c r="C129" t="n">
-        <v>1</v>
-      </c>
+      <c r="C129"/>
       <c r="D129"/>
       <c r="E129"/>
     </row>
@@ -3354,9 +3274,7 @@
       <c r="B130" t="n">
         <v>0</v>
       </c>
-      <c r="C130" t="n">
-        <v>1</v>
-      </c>
+      <c r="C130"/>
       <c r="D130"/>
       <c r="E130"/>
     </row>
@@ -3367,9 +3285,7 @@
       <c r="B131" t="n">
         <v>0</v>
       </c>
-      <c r="C131" t="n">
-        <v>1</v>
-      </c>
+      <c r="C131"/>
       <c r="D131"/>
       <c r="E131"/>
     </row>
@@ -3380,9 +3296,7 @@
       <c r="B132" t="n">
         <v>0</v>
       </c>
-      <c r="C132" t="n">
-        <v>1</v>
-      </c>
+      <c r="C132"/>
       <c r="D132" t="s">
         <v>13</v>
       </c>
@@ -3421,9 +3335,7 @@
       <c r="B135" t="n">
         <v>0</v>
       </c>
-      <c r="C135" t="n">
-        <v>1</v>
-      </c>
+      <c r="C135"/>
       <c r="D135"/>
       <c r="E135"/>
     </row>
@@ -3434,9 +3346,7 @@
       <c r="B136" t="n">
         <v>0</v>
       </c>
-      <c r="C136" t="n">
-        <v>1</v>
-      </c>
+      <c r="C136"/>
       <c r="D136"/>
       <c r="E136"/>
     </row>
@@ -3447,9 +3357,7 @@
       <c r="B137" t="n">
         <v>0</v>
       </c>
-      <c r="C137" t="n">
-        <v>1</v>
-      </c>
+      <c r="C137"/>
       <c r="D137"/>
       <c r="E137"/>
     </row>
@@ -3486,9 +3394,7 @@
       <c r="B140" t="n">
         <v>0</v>
       </c>
-      <c r="C140" t="n">
-        <v>1</v>
-      </c>
+      <c r="C140"/>
       <c r="D140"/>
       <c r="E140"/>
     </row>
@@ -3499,9 +3405,7 @@
       <c r="B141" t="n">
         <v>0</v>
       </c>
-      <c r="C141" t="n">
-        <v>1</v>
-      </c>
+      <c r="C141"/>
       <c r="D141"/>
       <c r="E141"/>
     </row>
@@ -3538,9 +3442,7 @@
       <c r="B144" t="n">
         <v>0</v>
       </c>
-      <c r="C144" t="n">
-        <v>0</v>
-      </c>
+      <c r="C144"/>
       <c r="D144"/>
       <c r="E144"/>
     </row>
@@ -3551,9 +3453,7 @@
       <c r="B145" t="n">
         <v>0</v>
       </c>
-      <c r="C145" t="n">
-        <v>0</v>
-      </c>
+      <c r="C145"/>
       <c r="D145"/>
       <c r="E145"/>
     </row>
@@ -3577,9 +3477,7 @@
       <c r="B147" t="n">
         <v>0</v>
       </c>
-      <c r="C147" t="n">
-        <v>1</v>
-      </c>
+      <c r="C147"/>
       <c r="D147" t="s">
         <v>9</v>
       </c>
@@ -3592,9 +3490,7 @@
       <c r="B148" t="n">
         <v>0</v>
       </c>
-      <c r="C148" t="n">
-        <v>1</v>
-      </c>
+      <c r="C148"/>
       <c r="D148"/>
       <c r="E148"/>
     </row>
@@ -3618,9 +3514,7 @@
       <c r="B150" t="n">
         <v>0</v>
       </c>
-      <c r="C150" t="n">
-        <v>1</v>
-      </c>
+      <c r="C150"/>
       <c r="D150"/>
       <c r="E150"/>
     </row>
@@ -3631,9 +3525,7 @@
       <c r="B151" t="n">
         <v>0</v>
       </c>
-      <c r="C151" t="n">
-        <v>1</v>
-      </c>
+      <c r="C151"/>
       <c r="D151"/>
       <c r="E151"/>
     </row>
@@ -3644,9 +3536,7 @@
       <c r="B152" t="n">
         <v>0</v>
       </c>
-      <c r="C152" t="n">
-        <v>1</v>
-      </c>
+      <c r="C152"/>
       <c r="D152"/>
       <c r="E152"/>
     </row>
@@ -3670,9 +3560,7 @@
       <c r="B154" t="n">
         <v>0</v>
       </c>
-      <c r="C154" t="n">
-        <v>0</v>
-      </c>
+      <c r="C154"/>
       <c r="D154"/>
       <c r="E154"/>
     </row>
@@ -3709,9 +3597,7 @@
       <c r="B157" t="n">
         <v>0</v>
       </c>
-      <c r="C157" t="n">
-        <v>1</v>
-      </c>
+      <c r="C157"/>
       <c r="D157"/>
       <c r="E157"/>
     </row>
@@ -3820,9 +3706,7 @@
       <c r="B164" t="n">
         <v>0</v>
       </c>
-      <c r="C164" t="n">
-        <v>0</v>
-      </c>
+      <c r="C164"/>
       <c r="D164"/>
       <c r="E164"/>
     </row>
@@ -3931,9 +3815,7 @@
       <c r="B171" t="n">
         <v>0</v>
       </c>
-      <c r="C171" t="n">
-        <v>0</v>
-      </c>
+      <c r="C171"/>
       <c r="D171"/>
       <c r="E171"/>
     </row>
@@ -4038,9 +3920,7 @@
       <c r="B178" t="n">
         <v>0</v>
       </c>
-      <c r="C178" t="n">
-        <v>0</v>
-      </c>
+      <c r="C178"/>
       <c r="D178"/>
       <c r="E178"/>
     </row>
@@ -4153,9 +4033,7 @@
       <c r="B185" t="n">
         <v>0</v>
       </c>
-      <c r="C185" t="n">
-        <v>0</v>
-      </c>
+      <c r="C185"/>
       <c r="D185" t="s">
         <v>9</v>
       </c>
@@ -4168,9 +4046,7 @@
       <c r="B186" t="n">
         <v>0</v>
       </c>
-      <c r="C186" t="n">
-        <v>0</v>
-      </c>
+      <c r="C186"/>
       <c r="D186" t="s">
         <v>9</v>
       </c>
@@ -4264,9 +4140,7 @@
       <c r="B192" t="n">
         <v>0</v>
       </c>
-      <c r="C192" t="n">
-        <v>0</v>
-      </c>
+      <c r="C192"/>
       <c r="D192"/>
       <c r="E192"/>
     </row>
@@ -4307,9 +4181,7 @@
       <c r="B195" t="n">
         <v>0</v>
       </c>
-      <c r="C195" t="n">
-        <v>0</v>
-      </c>
+      <c r="C195"/>
       <c r="D195"/>
       <c r="E195"/>
     </row>
@@ -4354,9 +4226,7 @@
       <c r="B198" t="n">
         <v>0</v>
       </c>
-      <c r="C198" t="n">
-        <v>0</v>
-      </c>
+      <c r="C198"/>
       <c r="D198" t="s">
         <v>15</v>
       </c>
@@ -4386,9 +4256,7 @@
       <c r="B200" t="n">
         <v>0</v>
       </c>
-      <c r="C200" t="n">
-        <v>0</v>
-      </c>
+      <c r="C200"/>
       <c r="D200"/>
       <c r="E200"/>
     </row>
@@ -4497,9 +4365,7 @@
       <c r="B207" t="n">
         <v>0</v>
       </c>
-      <c r="C207" t="n">
-        <v>0</v>
-      </c>
+      <c r="C207"/>
       <c r="D207" t="s">
         <v>9</v>
       </c>
@@ -4682,9 +4548,7 @@
       <c r="B218" t="n">
         <v>0</v>
       </c>
-      <c r="C218" t="n">
-        <v>0</v>
-      </c>
+      <c r="C218"/>
       <c r="D218" t="s">
         <v>15</v>
       </c>
@@ -4850,9 +4714,7 @@
       <c r="B228" t="n">
         <v>0</v>
       </c>
-      <c r="C228" t="n">
-        <v>0</v>
-      </c>
+      <c r="C228"/>
       <c r="D228" t="s">
         <v>6</v>
       </c>
@@ -5001,9 +4863,7 @@
       <c r="B237" t="n">
         <v>0</v>
       </c>
-      <c r="C237" t="n">
-        <v>0</v>
-      </c>
+      <c r="C237"/>
       <c r="D237" t="s">
         <v>6</v>
       </c>
@@ -5016,9 +4876,7 @@
       <c r="B238" t="n">
         <v>0</v>
       </c>
-      <c r="C238" t="n">
-        <v>0</v>
-      </c>
+      <c r="C238"/>
       <c r="D238"/>
       <c r="E238"/>
     </row>
@@ -5029,9 +4887,7 @@
       <c r="B239" t="n">
         <v>0</v>
       </c>
-      <c r="C239" t="n">
-        <v>0</v>
-      </c>
+      <c r="C239"/>
       <c r="D239"/>
       <c r="E239"/>
     </row>
@@ -5042,9 +4898,7 @@
       <c r="B240" t="n">
         <v>0</v>
       </c>
-      <c r="C240" t="n">
-        <v>0</v>
-      </c>
+      <c r="C240"/>
       <c r="D240"/>
       <c r="E240"/>
     </row>
@@ -5068,9 +4922,7 @@
       <c r="B242" t="n">
         <v>0</v>
       </c>
-      <c r="C242" t="n">
-        <v>0</v>
-      </c>
+      <c r="C242"/>
       <c r="D242" t="s">
         <v>13</v>
       </c>
@@ -5168,9 +5020,7 @@
       <c r="B248" t="n">
         <v>0</v>
       </c>
-      <c r="C248" t="n">
-        <v>1</v>
-      </c>
+      <c r="C248"/>
       <c r="D248"/>
       <c r="E248"/>
     </row>
@@ -5181,9 +5031,7 @@
       <c r="B249" t="n">
         <v>0</v>
       </c>
-      <c r="C249" t="n">
-        <v>1</v>
-      </c>
+      <c r="C249"/>
       <c r="D249" t="s">
         <v>9</v>
       </c>
@@ -5230,9 +5078,7 @@
       <c r="B252" t="n">
         <v>0</v>
       </c>
-      <c r="C252" t="n">
-        <v>0</v>
-      </c>
+      <c r="C252"/>
       <c r="D252" t="s">
         <v>9</v>
       </c>
@@ -5394,9 +5240,7 @@
       <c r="B262" t="n">
         <v>0</v>
       </c>
-      <c r="C262" t="n">
-        <v>0</v>
-      </c>
+      <c r="C262"/>
       <c r="D262" t="s">
         <v>6</v>
       </c>
@@ -5579,9 +5423,7 @@
       <c r="B273" t="n">
         <v>0</v>
       </c>
-      <c r="C273" t="n">
-        <v>0</v>
-      </c>
+      <c r="C273"/>
       <c r="D273"/>
       <c r="E273"/>
     </row>
@@ -5677,9 +5519,7 @@
       <c r="B279" t="n">
         <v>0</v>
       </c>
-      <c r="C279" t="n">
-        <v>0</v>
-      </c>
+      <c r="C279"/>
       <c r="D279"/>
       <c r="E279"/>
     </row>
@@ -5758,9 +5598,7 @@
       <c r="B284" t="n">
         <v>0</v>
       </c>
-      <c r="C284" t="n">
-        <v>0</v>
-      </c>
+      <c r="C284"/>
       <c r="D284"/>
       <c r="E284"/>
     </row>
@@ -5822,9 +5660,7 @@
       <c r="B288" t="n">
         <v>0</v>
       </c>
-      <c r="C288" t="n">
-        <v>0</v>
-      </c>
+      <c r="C288"/>
       <c r="D288" t="s">
         <v>6</v>
       </c>
@@ -5884,9 +5720,7 @@
       <c r="B292" t="n">
         <v>0</v>
       </c>
-      <c r="C292" t="n">
-        <v>0</v>
-      </c>
+      <c r="C292"/>
       <c r="D292" t="s">
         <v>9</v>
       </c>
@@ -6185,9 +6019,7 @@
       <c r="B311" t="n">
         <v>0</v>
       </c>
-      <c r="C311" t="n">
-        <v>0</v>
-      </c>
+      <c r="C311"/>
       <c r="D311" t="s">
         <v>6</v>
       </c>
@@ -6234,9 +6066,7 @@
       <c r="B314" t="n">
         <v>0</v>
       </c>
-      <c r="C314" t="n">
-        <v>0</v>
-      </c>
+      <c r="C314"/>
       <c r="D314" t="s">
         <v>6</v>
       </c>

</xml_diff>